<commit_message>
A number of changes and fixes to Rtd support to allow async rtd tasks to work correctly with multiple task in the same cell.   Still needs more polish and a lot more comments.
Add Rtd async functions to python. These work a lot more naturally than Excel's built in asyncs, but with the overheads of the Rtd machinery and the comparison of tasks.

Updated the RtdTest sheet and the python test sheet to use the Rtd functions
</commit_message>
<xml_diff>
--- a/tests/rtd/RtdTest.xlsx
+++ b/tests/rtd/RtdTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\rtd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{88253639-5B04-4237-A42D-D59AD3B8D612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E890F4-B7B5-4B22-BA91-CACCB4191FEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="948" yWindow="-108" windowWidth="22200" windowHeight="13176"/>
+    <workbookView xWindow="948" yWindow="-108" windowWidth="22200" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>X</t>
   </si>
@@ -44,11 +44,17 @@
   <si>
     <t>Counter</t>
   </si>
+  <si>
+    <t>Skip</t>
+  </si>
+  <si>
+    <t>Skip+1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,6 +132,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
+<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <volType type="realTimeData">
+    <main first="xloil.rtd.44671cf2.a667.467e.ad59.b8957fa6f64f">
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>X</stp>
+        <tr r="C7" s="1"/>
+        <tr r="C6" s="1"/>
+        <tr r="C5" s="1"/>
+      </tp>
+    </main>
+    <main first="xloil.rtd.01d1e87e.6461.41f1.aebf.523bba6d33c2">
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>{9CC46D94-FCF2-4C86-BBF6-7AB4952DAB4F}</stp>
+        <tr r="F13" s="1"/>
+      </tp>
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>{B0228C62-2874-44FD-AC8F-1200E22DC219}</stp>
+        <tr r="F13" s="1"/>
+      </tp>
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>{CE15D0C5-04FA-4AAC-A8A3-40211E8D5C9E}</stp>
+        <tr r="F8" s="1"/>
+      </tp>
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>{7957877F-466B-4F54-861F-06F72EDB7231}</stp>
+        <tr r="F5" s="1"/>
+      </tp>
+      <tp>
+        <v>0</v>
+        <stp/>
+        <stp>{2970BFAD-2392-4935-A8A5-F90ADB66637A}</stp>
+        <tr r="F13" s="1"/>
+      </tp>
+    </main>
+  </volType>
+</volTypes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -424,11 +479,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="B3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,7 +492,7 @@
     <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -445,7 +501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -454,51 +510,78 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="e">
-        <f t="array" aca="1" ref="C5:C7" ca="1">_xll.xloRtdGet(B3)</f>
-        <v>#VALUE!</v>
+      <c r="C5" s="4">
+        <f t="array" ref="C5:C7">_xll.xloRtdGet(B3)</f>
+        <v>1</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" t="e">
-        <f ca="1">_xll.xloRtdCounter()</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4">
+        <f>_xll.xloRtdCounter()</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
+      <c r="C6" s="4">
+        <v>2</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" t="e">
-        <f ca="1">_xll.xloRtdCounter()+1</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="e">
-        <f ca="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E7" t="e">
-        <f ca="1">_xll.xloRtdCounter()</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="e">
-        <f ca="1">_xll.xloRtdSet(B3,B5:B7)</f>
-        <v>#VALUE!</v>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="str">
+        <f>_xll.xloRtdSet(B3,B5:B7)</f>
+        <v>X</v>
+      </c>
+      <c r="F8" s="4">
+        <f>_xll.xloRtdCounter(F7)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F13" s="4">
+        <f>_xll.xloRtdCounter(F10)+_xll.xloRtdCounter(F11)+_xll.xloRtdCounter(F12)</f>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>